<commit_message>
create xlreader and implement
</commit_message>
<xml_diff>
--- a/placeholder.xlsx
+++ b/placeholder.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luked\Documents\schemaChecker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1B12B9BB-DAA1-4DAF-A18E-63CA6821AD90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29518EB4-C459-478C-8435-826C628E1440}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{421BA4EB-5B89-4FFE-94B6-28149CFF3C9B}"/>
   </bookViews>
@@ -38,18 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
-    <t>First Name</t>
-  </si>
-  <si>
-    <t>Last Name</t>
-  </si>
-  <si>
-    <t>Emp_ID</t>
-  </si>
-  <si>
-    <t>Wage</t>
-  </si>
-  <si>
     <t>Max</t>
   </si>
   <si>
@@ -96,6 +84,18 @@
   </si>
   <si>
     <t>Piastri</t>
+  </si>
+  <si>
+    <t>first_name</t>
+  </si>
+  <si>
+    <t>last_name</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>wage</t>
   </si>
 </sst>
 </file>
@@ -449,9 +449,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3A3EB0D-50BF-4D97-9BF4-FF8544AB9AB6}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -460,24 +458,24 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>25562</v>
@@ -488,10 +486,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C3">
         <v>55652</v>
@@ -502,10 +500,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C4">
         <v>36656</v>
@@ -516,10 +514,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C5">
         <v>78852</v>
@@ -530,10 +528,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C6">
         <v>98952</v>
@@ -544,10 +542,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C7">
         <v>74522</v>
@@ -558,10 +556,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C8">
         <v>56897</v>
@@ -572,10 +570,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C9">
         <v>86598</v>

</xml_diff>